<commit_message>
section 5 - functions
</commit_message>
<xml_diff>
--- a/Final Project -- Budget Workbook.xlsx
+++ b/Final Project -- Budget Workbook.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joemacbook/Desktop/ZTM_Excel_Bootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F001E54F-565B-D24D-9047-FF780EFA53B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F4610D-F88F-CB4B-A646-1E64550912FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="660" windowWidth="28040" windowHeight="19900" xr2:uid="{9304599E-7F71-2640-9DD6-7DBF4C601D9D}"/>
+    <workbookView xWindow="1180" yWindow="820" windowWidth="28040" windowHeight="19900" xr2:uid="{9304599E-7F71-2640-9DD6-7DBF4C601D9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly Income" sheetId="2" r:id="rId2"/>
+    <sheet name="Monthly Expenses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Budget and Expense Summary</t>
   </si>
@@ -47,6 +49,60 @@
   </si>
   <si>
     <t xml:space="preserve">Cash Balance: </t>
+  </si>
+  <si>
+    <t>Side Hustle 1</t>
+  </si>
+  <si>
+    <t>Income 2</t>
+  </si>
+  <si>
+    <t>Income 1</t>
+  </si>
+  <si>
+    <t>Estimated Amount</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Phone/Cable</t>
+  </si>
+  <si>
+    <t>Dining</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Home Insurance</t>
+  </si>
+  <si>
+    <t>Auto Insurance</t>
+  </si>
+  <si>
+    <t>Auto repair/maintenance</t>
+  </si>
+  <si>
+    <t>Car payment</t>
+  </si>
+  <si>
+    <t>Groceries</t>
+  </si>
+  <si>
+    <t>Cell phone</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Rent/Mortgage</t>
   </si>
 </sst>
 </file>
@@ -56,7 +112,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +172,26 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -145,36 +228,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{54F01130-99E6-6D47-948A-DD395D98338D}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -405,7 +498,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,7 +524,8 @@
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>2</v>
+        <f>SUM('Monthly Income'!B2:B4)</f>
+        <v>7606</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="11" customHeight="1" x14ac:dyDescent="0.2">
@@ -443,7 +537,8 @@
         <v>2</v>
       </c>
       <c r="C5" s="6">
-        <v>1</v>
+        <f>SUM('Monthly Expenses'!B2:B14)</f>
+        <v>5668</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -456,7 +551,7 @@
       </c>
       <c r="C7" s="7">
         <f>C3-C5</f>
-        <v>1</v>
+        <v>1938</v>
       </c>
     </row>
   </sheetData>
@@ -470,4 +565,189 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735ECDE8-DA2A-D64E-873F-FFA77B5BADF7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="206" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="10">
+        <v>3026</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89781B2A-0BE2-8D4D-A301-7B6EC4E0515F}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView zoomScale="176" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="12">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="12">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="12">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>